<commit_message>
Add new Excel figures
</commit_message>
<xml_diff>
--- a/saved_results/Tests/UPM-GTI-Face/Mask/AUC Curves.xlsx
+++ b/saved_results/Tests/UPM-GTI-Face/Mask/AUC Curves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Doctorado UPM\Papers\Paper ViT\ViT-Face-Recognition\saved_results\Tests\UPM-GTI-Face\Mask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F91C5E-A091-4258-942B-93365F13EE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F570E245-4C5D-4991-BDEF-92256EF28550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12840" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3309,6 +3309,1026 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl" sz="2000"/>
+              <a:t>Area Under</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl" sz="2000" baseline="0"/>
+              <a:t> the Curve (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl" sz="2000"/>
+              <a:t>AUC)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ViT_B32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ResNet_50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VGG_16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>InceptionNet_V3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00FFFF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FFFF"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00FFFF"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MobileNet_V2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="CC0099"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="CC0099"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="CC0099"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$4:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EfficientNet_B0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FCF3-45B8-8C81-E1078D6ED618}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1728503648"/>
+        <c:axId val="1728501984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1728503648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1800"/>
+                  <a:t>Distance (meters)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1728501984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1728501984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1800"/>
+                  <a:t>AUC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1728503648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1756873130195914"/>
+          <c:y val="0.39384600388494106"/>
+          <c:w val="0.35136012528650318"/>
+          <c:h val="0.40575988183596839"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3429,6 +4449,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4436,6 +5496,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5049,6 +6612,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28291</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0267A51-22E6-4495-B26A-0C98F77F4A60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5322,8 +6923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="H18" zoomScale="101" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AH42" sqref="AH42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>